<commit_message>
Change Structure & Move Cur Unit to Level Data
</commit_message>
<xml_diff>
--- a/Assets/Excel/CharacterSkill.xlsx
+++ b/Assets/Excel/CharacterSkill.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23070" windowHeight="13040"/>
+    <workbookView windowWidth="25600" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="CharacterSkill" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>//Remark</t>
   </si>
@@ -28,13 +28,22 @@
     <t>desc</t>
   </si>
   <si>
+    <t>range</t>
+  </si>
+  <si>
+    <t>radius</t>
+  </si>
+  <si>
     <t>int</t>
   </si>
   <si>
     <t>string</t>
   </si>
   <si>
-    <t>Water</t>
+    <t>Elemental Bolt</t>
+  </si>
+  <si>
+    <t>Strike</t>
   </si>
 </sst>
 </file>
@@ -1002,13 +1011,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="4" outlineLevelCol="4"/>
   <cols>
     <col min="2" max="2" width="19.3636363636364" customWidth="1"/>
     <col min="3" max="3" width="15.5454545454545" customWidth="1"/>
@@ -1019,7 +1028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1029,34 +1038,56 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>11001</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
+      <c r="E4">
+        <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4">
-        <v>1001</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:5">
       <c r="A5">
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6">
-        <v>3001</v>
+        <v>21001</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Can Deal Damage to foes
</commit_message>
<xml_diff>
--- a/Assets/Excel/CharacterSkill.xlsx
+++ b/Assets/Excel/CharacterSkill.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t>//Remark</t>
   </si>
@@ -40,6 +40,9 @@
     <t>regionType</t>
   </si>
   <si>
+    <t>isTargetFoe</t>
+  </si>
+  <si>
     <t>int</t>
   </si>
   <si>
@@ -50,6 +53,9 @@
   </si>
   <si>
     <t>enum|SkillRegionType</t>
+  </si>
+  <si>
+    <t>bool</t>
   </si>
   <si>
     <t>Elemental Ball</t>
@@ -1053,18 +1059,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="6" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="6" outlineLevelCol="7"/>
   <cols>
     <col min="2" max="2" width="19.3636363636364" customWidth="1"/>
     <col min="3" max="3" width="49" customWidth="1"/>
     <col min="4" max="4" width="22.4545454545455" customWidth="1"/>
     <col min="7" max="7" width="20.8181818181818" customWidth="1"/>
+    <col min="8" max="8" width="12.3636363636364" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1072,7 +1079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1094,42 +1101,48 @@
       <c r="G2" t="s">
         <v>7</v>
       </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="F3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" t="s">
-        <v>8</v>
-      </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="H3" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>1001</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E4">
         <v>4</v>
@@ -1138,21 +1151,24 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="H4" t="b">
+        <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8">
       <c r="A5">
         <v>1101</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -1161,21 +1177,24 @@
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="H5" t="b">
+        <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:8">
       <c r="A6">
         <v>2001</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -1184,21 +1203,24 @@
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="H6" t="b">
+        <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:8">
       <c r="A7">
         <v>2101</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -1207,7 +1229,10 @@
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>23</v>
+        <v>25</v>
+      </c>
+      <c r="H7" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>